<commit_message>
Code ready for hand in
</commit_message>
<xml_diff>
--- a/Zapojeni.xlsx
+++ b/Zapojeni.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHubRepos\CubeWorkspace\Semestralka2EMBEDDED\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EEC4DC8-8F8F-4906-81EF-C35868DF2912}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE883E99-1960-4661-99E2-D37B02B26101}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4044" yWindow="2388" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Zobackem nahoru</t>
   </si>
@@ -61,6 +61,21 @@
   </si>
   <si>
     <t>Q3</t>
+  </si>
+  <si>
+    <t>APB2</t>
+  </si>
+  <si>
+    <t>MHZ</t>
+  </si>
+  <si>
+    <t>APB1</t>
+  </si>
+  <si>
+    <t>timer</t>
+  </si>
+  <si>
+    <t>adc</t>
   </si>
 </sst>
 </file>
@@ -466,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:K6"/>
+  <dimension ref="C3:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -522,6 +537,48 @@
         <v>4</v>
       </c>
     </row>
+    <row r="8" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8">
+        <v>96</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="F16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16">
+        <v>500000</v>
+      </c>
+      <c r="I16">
+        <f>G17*122</f>
+        <v>499712</v>
+      </c>
+    </row>
+    <row r="17" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17">
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="19" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F19">
+        <f>G16/G17</f>
+        <v>122.0703125</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>